<commit_message>
updated .csv files with correct data, having foreign key problems
</commit_message>
<xml_diff>
--- a/usmart_energy_site/seed_files/asset_seed.xlsx
+++ b/usmart_energy_site/seed_files/asset_seed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pstewy/Documents/SeniorCollege/SeniorCapstoneProject/code/usmart-energy/usmart_energy_site/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonhansen/Documents/School/capstone/usmart-energy/usmart_energy_site/seed_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F59D1E5E-B06A-D146-B7DC-7F9A51154BF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC82996-4EE9-A946-8ECD-CEA6BABD9F7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="940" windowWidth="25040" windowHeight="14260"/>
+    <workbookView xWindow="20" yWindow="8240" windowWidth="25600" windowHeight="7760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="asset_seed" sheetId="1" r:id="rId1"/>
@@ -20,33 +20,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>Rman's Solar,,0.8</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Solar Panel</t>
   </si>
   <si>
-    <t>SolarP,0.3</t>
+    <t>USmart Charger</t>
   </si>
   <si>
-    <t>Wind turbine</t>
+    <t>Backyard Solar Panel</t>
   </si>
   <si>
-    <t>WindT</t>
+    <t xml:space="preserve">Roof Wind Turbine </t>
   </si>
   <si>
-    <t>Mice Worker</t>
+    <t>Blue Tesla Model X</t>
   </si>
   <si>
-    <t>JradMiceWorker</t>
+    <t>Red Tesla Model 3</t>
+  </si>
+  <si>
+    <t>No preferences</t>
+  </si>
+  <si>
+    <t>Deadline: 07:00:00</t>
+  </si>
+  <si>
+    <t>Deadline: 06:30:00</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -524,8 +536,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -880,60 +893,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1">
+        <v>15</v>
+      </c>
+      <c r="E1">
+        <v>55</v>
+      </c>
+      <c r="F1">
+        <v>200</v>
+      </c>
+      <c r="G1" t="b">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>0.8</v>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>7.7</v>
+      </c>
+      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>0.2</v>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>110</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>0.9</v>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>6.6</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>75</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed booleans in asset_seed files
</commit_message>
<xml_diff>
--- a/usmart_energy_site/seed_files/asset_seed.xlsx
+++ b/usmart_energy_site/seed_files/asset_seed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonhansen/Documents/School/capstone/usmart-energy/usmart_energy_site/seed_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC82996-4EE9-A946-8ECD-CEA6BABD9F7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D292CAC2-391E-C14D-9E9E-90E120A3E1CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="8240" windowWidth="25600" windowHeight="7760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8240" windowWidth="25600" windowHeight="7760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="asset_seed" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>Solar Panel</t>
   </si>
@@ -897,7 +897,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,8 +926,8 @@
       <c r="F1">
         <v>200</v>
       </c>
-      <c r="G1" t="b">
-        <v>1</v>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -958,8 +958,8 @@
       <c r="F2">
         <v>100</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -990,8 +990,8 @@
       <c r="F3">
         <v>110</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -1022,8 +1022,8 @@
       <c r="F4">
         <v>75</v>
       </c>
-      <c r="G4" t="b">
-        <v>0</v>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>

</xml_diff>